<commit_message>
Uploaded 05-九月-2019 17:00:58 {/src/main/resources/com/redhat/prudential_poc/Reject.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Reject.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Reject.xlsx
@@ -1,30 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA330731-85D6-EC4C-BAC9-86359D3A330C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="15960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId4"/>
+    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>RuleSet</t>
   </si>
   <si>
-    <t>com.myspace.rules</t>
-  </si>
-  <si>
     <t>Import</t>
   </si>
   <si>
-    <t>com.myspace.Application,com.myspace.Insured</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -80,44 +83,71 @@
   </si>
   <si>
     <t>Z223456123</t>
+  </si>
+  <si>
+    <t>com.redhat.prudential_poc.rules</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.redhat.prudential_poc.pojo.Application,com.redhat.prudential_poc.pojo.Insured</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="新細明體"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="新細明體"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Wawati TC"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +178,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -160,62 +196,6 @@
     <border>
       <left style="hair">
         <color indexed="8"/>
-      </left>
-      <right style="hair">
-        <color indexed="8"/>
-      </right>
-      <top style="hair">
-        <color indexed="8"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color indexed="8"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="hair">
-        <color indexed="8"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="hair">
-        <color indexed="8"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
       </left>
       <right style="hair">
         <color indexed="8"/>
@@ -385,123 +365,210 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffcc"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffff6633"/>
-      <rgbColor rgb="ff94bd5e"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFFF6633"/>
+      <rgbColor rgb="FF94BD5E"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office 佈景主題">
       <a:dk1>
@@ -703,7 +770,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -722,7 +789,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -752,7 +819,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -778,7 +845,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -804,7 +871,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -830,7 +897,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -856,7 +923,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -882,7 +949,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -908,7 +975,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -934,7 +1001,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -960,7 +1027,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -973,9 +1040,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -992,7 +1065,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1011,7 +1084,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1037,7 +1110,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1063,7 +1136,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1089,7 +1162,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1115,7 +1188,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1141,7 +1214,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1167,7 +1240,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1193,7 +1266,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1219,7 +1292,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1245,7 +1318,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1258,9 +1331,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1274,7 +1353,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1293,7 +1372,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1323,7 +1402,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1349,7 +1428,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1375,7 +1454,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1401,7 +1480,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1427,7 +1506,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1453,7 +1532,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1479,7 +1558,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1505,7 +1584,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1531,7 +1610,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1544,178 +1623,185 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:IV11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.8516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.8516" style="1" customWidth="1"/>
-    <col min="7" max="256" width="10.8516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" style="1" customWidth="1"/>
+    <col min="7" max="256" width="10.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" s="28" customFormat="1" ht="16">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" s="28" customFormat="1" ht="16">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
+      <c r="B2" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
     </row>
-    <row r="2" ht="16" customHeight="1">
-      <c r="A2" t="s" s="7">
+    <row r="3" spans="1:7" ht="16" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
     </row>
-    <row r="3" ht="16" customHeight="1">
-      <c r="A3" t="s" s="2">
+    <row r="4" spans="1:7" ht="17" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="16" customHeight="1">
+      <c r="A5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" customHeight="1">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="9"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+    <row r="7" spans="1:7" ht="17" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="9"/>
     </row>
-    <row r="5" ht="16" customHeight="1">
-      <c r="A5" t="s" s="13">
-        <v>6</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+    <row r="8" spans="1:7" ht="17" customHeight="1">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="9"/>
     </row>
-    <row r="6" ht="16" customHeight="1">
-      <c r="A6" t="s" s="17">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s" s="17">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s" s="18">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="16"/>
+    <row r="9" spans="1:7" ht="17" customHeight="1">
+      <c r="A9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="9"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="16"/>
+    <row r="10" spans="1:7" ht="16" customHeight="1">
+      <c r="A10" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="9"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
-      <c r="A8" s="22"/>
-      <c r="B8" t="s" s="23">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s" s="23">
-        <v>13</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" t="s" s="24">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s" s="24">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s" s="25">
-        <v>16</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" ht="16" customHeight="1">
-      <c r="A10" t="s" s="26">
+    <row r="11" spans="1:7" ht="16" customHeight="1">
+      <c r="A11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s" s="17">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s" s="19">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s" s="19">
-        <v>20</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" ht="16" customHeight="1">
-      <c r="A11" t="s" s="26">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s" s="17">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s" s="19">
-        <v>19</v>
-      </c>
       <c r="D11" s="21"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="16"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
+  <mergeCells count="2">
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="A5:C5"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 18:32:30 {/src/main/resources/com/redhat/prudential_poc/Reject.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Reject.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Reject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA330731-85D6-EC4C-BAC9-86359D3A330C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FB3BB6-5E0C-BB44-8486-5414A62BEB46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="15960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>$insured: Insured</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>$insured.setStatus($param);</t>
   </si>
   <si>
@@ -86,10 +83,14 @@
   </si>
   <si>
     <t>com.redhat.prudential_poc.rules</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.redhat.prudential_poc.pojo.Application,com.redhat.prudential_poc.pojo.Insured</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.redhat.prudential_poc.pojo.Insured</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>insuredId</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -97,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -115,6 +116,13 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
     </font>
     <font>
       <sz val="12"/>
@@ -399,7 +407,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -469,18 +477,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1645,7 +1656,7 @@
   <dimension ref="A1:IV11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -1664,7 +1675,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
@@ -1677,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -1740,11 +1751,11 @@
     </row>
     <row r="8" spans="1:7" ht="17" customHeight="1">
       <c r="A8" s="15"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>10</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>11</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="13"/>
@@ -1752,13 +1763,13 @@
     </row>
     <row r="9" spans="1:7" ht="17" customHeight="1">
       <c r="A9" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="C9" s="18" t="s">
         <v>13</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>14</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="13"/>
@@ -1766,29 +1777,29 @@
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1">
       <c r="A10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="D10" s="20" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>18</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="16" customHeight="1">
       <c r="A11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>20</v>
-      </c>
       <c r="C11" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="13"/>
@@ -1799,7 +1810,7 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="A5:C5"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
Uploaded 06-九月-2019 00:13:18 {/src/main/resources/com/redhat/prudential_poc/Reject.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/Reject.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/Reject.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FB3BB6-5E0C-BB44-8486-5414A62BEB46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDBDF9A-8055-5A42-8560-BE6A7278CE14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="15960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>reject-rule1</t>
   </si>
   <si>
-    <t>A223456123</t>
-  </si>
-  <si>
     <t>"拒保"</t>
   </si>
   <si>
@@ -91,6 +88,10 @@
   </si>
   <si>
     <t>insuredId</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>A223456789</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -464,6 +465,22 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -475,22 +492,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1656,7 +1657,7 @@
   <dimension ref="A1:IV11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -1670,28 +1671,28 @@
     <col min="7" max="256" width="10.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="28" customFormat="1" ht="16">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:7" s="23" customFormat="1" ht="16">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" s="23" customFormat="1" ht="16">
+      <c r="A2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-    </row>
-    <row r="2" spans="1:7" s="28" customFormat="1" ht="16">
-      <c r="A2" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1714,11 +1715,11 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:7" ht="16" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -1751,8 +1752,8 @@
     </row>
     <row r="8" spans="1:7" ht="17" customHeight="1">
       <c r="A8" s="15"/>
-      <c r="B8" s="30" t="s">
-        <v>22</v>
+      <c r="B8" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>10</v>
@@ -1780,28 +1781,28 @@
         <v>14</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="D10" s="26" t="s">
         <v>16</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>17</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="16" customHeight="1">
       <c r="A11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="21"/>
+        <v>15</v>
+      </c>
+      <c r="D11" s="27"/>
       <c r="E11" s="13"/>
       <c r="F11" s="9"/>
     </row>

</xml_diff>